<commit_message>
Excel file after merging and manipulating data
</commit_message>
<xml_diff>
--- a/Data_with_Coordinates.xlsx
+++ b/Data_with_Coordinates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenzaelhoussaini/code/kelhoussaini/data_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C67421F-4AA9-E243-8AAB-FA2BA10BB189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDB447D-D2BF-D04C-8BB7-36D5C7E59775}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="2400" windowWidth="28800" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3568,6 +3568,7 @@
   <cols>
     <col min="5" max="5" width="22.83203125" customWidth="1"/>
     <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="18.5" customWidth="1"/>
     <col min="9" max="9" width="29.33203125" customWidth="1"/>
   </cols>

</xml_diff>